<commit_message>
Separates tests from project framework
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lavan\Desktop\LavanyaIC\StandardTask\marsproject\MarsFramework\ExcelData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55684B7-B47B-42A2-8F0B-A2B00A64C0E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" activeTab="6"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="3" r:id="rId1"/>
@@ -20,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="94">
-  <si>
-    <t>Url</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="92">
   <si>
     <t>Username</t>
   </si>
@@ -227,10 +230,6 @@
   </si>
   <si>
     <t>SydneyQa2018</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://192.168.99.100:5000/</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -369,16 +368,16 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="177" formatCode="hh:mm:ss;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="hh:mm:ss;@"/>
   </numFmts>
   <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -391,7 +390,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -449,12 +448,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -462,8 +461,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -479,7 +478,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -521,7 +520,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -553,9 +552,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -587,6 +604,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -762,307 +797,293 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.875" customWidth="1"/>
-    <col min="2" max="2" width="22.75" customWidth="1"/>
-    <col min="3" max="3" width="27.875" customWidth="1"/>
-    <col min="4" max="4" width="18.625" customWidth="1"/>
-    <col min="5" max="5" width="27.875" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15">
-      <c r="A2" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="45.875" customWidth="1"/>
-    <col min="2" max="2" width="27.625" customWidth="1"/>
-    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15">
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15">
-      <c r="A3" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="11">
+      <c r="B3" s="11">
         <v>20182018</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2" display="Test@123"/>
-    <hyperlink ref="B2" r:id="rId3"/>
-    <hyperlink ref="B3" r:id="rId4"/>
-    <hyperlink ref="A3" r:id="rId5"/>
+    <hyperlink ref="B2" r:id="rId1" display="Test@123" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="20.125" customWidth="1"/>
-    <col min="5" max="5" width="18.25" customWidth="1"/>
-    <col min="6" max="6" width="24.875" customWidth="1"/>
+    <col min="1" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="12" width="12.75" customWidth="1"/>
-    <col min="13" max="13" width="17.125" customWidth="1"/>
-    <col min="14" max="14" width="19.625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.375" customWidth="1"/>
-    <col min="16" max="16" width="13.25" customWidth="1"/>
-    <col min="17" max="17" width="10.75" customWidth="1"/>
+    <col min="8" max="12" width="12.7109375" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" customWidth="1"/>
+    <col min="14" max="14" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.42578125" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" customWidth="1"/>
+    <col min="17" max="17" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="R1" s="1"/>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
         <v>41</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>42</v>
       </c>
-      <c r="E2" t="s">
-        <v>43</v>
-      </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K2" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="L2" s="10" t="s">
-        <v>49</v>
-      </c>
       <c r="M2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O2">
         <v>5</v>
       </c>
       <c r="P2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I3" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M3" t="s">
         <v>51</v>
       </c>
-      <c r="J3" t="s">
-        <v>46</v>
-      </c>
-      <c r="K3" t="s">
-        <v>47</v>
-      </c>
-      <c r="L3" t="s">
-        <v>50</v>
-      </c>
-      <c r="M3" t="s">
-        <v>52</v>
-      </c>
       <c r="N3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O3">
         <v>5</v>
       </c>
       <c r="P3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -1076,33 +1097,33 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.25" customWidth="1"/>
-    <col min="2" max="2" width="21.625" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="14.375" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="5" customFormat="1">
+    <row r="1" spans="1:17" s="5" customFormat="1" ht="13.5">
       <c r="A1" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
@@ -1118,18 +1139,18 @@
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
     </row>
-    <row r="2" spans="1:17" s="5" customFormat="1">
+    <row r="2" spans="1:17" s="5" customFormat="1" ht="13.5">
       <c r="A2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>37</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="7"/>
@@ -1145,56 +1166,56 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.125" customWidth="1"/>
-    <col min="2" max="2" width="17.375" customWidth="1"/>
-    <col min="3" max="3" width="22.5" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
         <v>63</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>65</v>
-      </c>
-      <c r="C3" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1205,26 +1226,26 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.375" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1234,101 +1255,101 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="23.5" customWidth="1"/>
-    <col min="3" max="3" width="18.625" customWidth="1"/>
-    <col min="4" max="4" width="21.875" customWidth="1"/>
-    <col min="5" max="5" width="20.125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" t="s">
         <v>80</v>
-      </c>
-      <c r="B2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" t="s">
         <v>84</v>
       </c>
-      <c r="C3" t="s">
-        <v>86</v>
-      </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>